<commit_message>
few task are completed
</commit_message>
<xml_diff>
--- a/issue-list.xlsx
+++ b/issue-list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mobile_Application\2024\drive-lingua-app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MobileApplication\2024\drive-lingua\drive-lingua-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE96B437-2FC0-4202-A3EC-6708B92E91AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4884148-5E50-4337-9572-CEF4DE9EB039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t xml:space="preserve">Issue </t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>all the button are hide now only language is showing</t>
+  </si>
+  <si>
+    <t>you can take care of this</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,16 +446,25 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -462,6 +474,9 @@
     <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>